<commit_message>
Fixed and updated broken dependencies.  The tests are like an overgrown garden.  They are seriously in need of a refactor.  Have to do this before I complete the Trello integration which is currently on a branch waiting to come in.
</commit_message>
<xml_diff>
--- a/jlf_stats/test/data/reports.xlsx
+++ b/jlf_stats/test/data/reports.xlsx
@@ -99,12 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -423,11 +422,10 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -435,13 +433,13 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -449,13 +447,13 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>